<commit_message>
cambios fichajes por resgitros
</commit_message>
<xml_diff>
--- a/backend/uploads/HORAS POR TRABAJADOR Y DIA  (10).xlsx
+++ b/backend/uploads/HORAS POR TRABAJADOR Y DIA  (10).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aljimenezl\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acciona365-my.sharepoint.com/personal/plinero_acciona_com/Documents/Documentos/PRACTICAS ACCIONA/FICHAJES-ALBA/BI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04E8A7B5-B764-438C-B1DA-FA51132E2FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{04E8A7B5-B764-438C-B1DA-FA51132E2FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEED5A76-CAC5-43A6-871E-68F1094E43FF}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
@@ -544,9 +544,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:P14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="28.6328125" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="4" max="4" width="28.6328125" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">

</xml_diff>

<commit_message>
Arreglado errores de cors
</commit_message>
<xml_diff>
--- a/backend/uploads/HORAS POR TRABAJADOR Y DIA  (10).xlsx
+++ b/backend/uploads/HORAS POR TRABAJADOR Y DIA  (10).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acciona365-my.sharepoint.com/personal/plinero_acciona_com/Documents/Documentos/PRACTICAS ACCIONA/FICHAJES-ALBA/BI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aljimenezl\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{04E8A7B5-B764-438C-B1DA-FA51132E2FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEED5A76-CAC5-43A6-871E-68F1094E43FF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04E8A7B5-B764-438C-B1DA-FA51132E2FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
@@ -544,19 +544,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:P14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="28.6328125" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="4" width="28.6328125" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" customWidth="1"/>
-    <col min="13" max="13" width="15.08984375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">

</xml_diff>

<commit_message>
Lee los dos archivos de excels
</commit_message>
<xml_diff>
--- a/backend/uploads/HORAS POR TRABAJADOR Y DIA  (10).xlsx
+++ b/backend/uploads/HORAS POR TRABAJADOR Y DIA  (10).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acciona365-my.sharepoint.com/personal/plinero_acciona_com/Documents/Documentos/PRACTICAS ACCIONA/FICHAJES-ALBA/BI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aljimenezl\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{04E8A7B5-B764-438C-B1DA-FA51132E2FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEED5A76-CAC5-43A6-871E-68F1094E43FF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04E8A7B5-B764-438C-B1DA-FA51132E2FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
@@ -544,19 +544,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:P14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="28.6328125" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="4" width="28.6328125" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" customWidth="1"/>
-    <col min="13" max="13" width="15.08984375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">

</xml_diff>

<commit_message>
Crea un resultado para el excel a descargar
</commit_message>
<xml_diff>
--- a/backend/uploads/HORAS POR TRABAJADOR Y DIA  (10).xlsx
+++ b/backend/uploads/HORAS POR TRABAJADOR Y DIA  (10).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acciona365-my.sharepoint.com/personal/plinero_acciona_com/Documents/Documentos/PRACTICAS ACCIONA/FICHAJES-ALBA/BI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acciona365-my.sharepoint.com/personal/vimunozca_acciona_com/Documents/Documentos/PRACTICAS ACCIONA/Bi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{04E8A7B5-B764-438C-B1DA-FA51132E2FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEED5A76-CAC5-43A6-871E-68F1094E43FF}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{04E8A7B5-B764-438C-B1DA-FA51132E2FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7173CF32-28E8-4393-90BE-0528EBC49E5E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -545,17 +545,14 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:P14"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="28.6328125" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="4" width="28.6328125" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" customWidth="1"/>
-    <col min="13" max="13" width="15.08984375" customWidth="1"/>
+    <col min="5" max="5" width="18.6328125" customWidth="1"/>
+    <col min="13" max="13" width="16.453125" customWidth="1"/>
+    <col min="14" max="14" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">

</xml_diff>